<commit_message>
Finalização do JAR v1 com logs, leitura e inserção de dados no banco
</commit_message>
<xml_diff>
--- a/leitor-base-de-dados-nexus/base de dados v1.xlsx
+++ b/leitor-base-de-dados-nexus/base de dados v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ventu\OneDrive\Documentos\Sptech\Projeto de PI\GitBash\Nexus\nexus-backend\leitor-base-de-dados-nexus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6630FCE-231A-48F6-A358-ACB4AA4B6914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAC1756B-A33C-40A1-B54F-2CF5DDD9B44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="456">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="820" uniqueCount="462">
   <si>
     <t>full_name</t>
   </si>
@@ -1387,14 +1387,32 @@
     <t>$145,728</t>
   </si>
   <si>
-    <t>31/06/2003</t>
+    <t>instagraminstagram</t>
+  </si>
+  <si>
+    <t>Regiao</t>
+  </si>
+  <si>
+    <t>América do Norte</t>
+  </si>
+  <si>
+    <t>Brasil</t>
+  </si>
+  <si>
+    <t>Elo divisao</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Challenger</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1429,6 +1447,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1438,7 +1464,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1461,6 +1487,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1469,7 +1506,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1478,7 +1515,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1784,28 +1825,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L69"/>
+  <dimension ref="A1:O69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" topLeftCell="H34" workbookViewId="0">
+      <selection activeCell="O84" sqref="O84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="47.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="42.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="42.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>234</v>
       </c>
@@ -1842,8 +1884,17 @@
       <c r="L1" s="1" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -1871,8 +1922,20 @@
       <c r="I2" s="2" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K2" t="s">
+        <v>455</v>
+      </c>
+      <c r="M2" t="s">
+        <v>457</v>
+      </c>
+      <c r="N2" t="s">
+        <v>460</v>
+      </c>
+      <c r="O2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1903,8 +1966,17 @@
       <c r="K3" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>457</v>
+      </c>
+      <c r="N3" t="s">
+        <v>460</v>
+      </c>
+      <c r="O3" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1938,8 +2010,17 @@
       <c r="L4" s="4" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>457</v>
+      </c>
+      <c r="N4" t="s">
+        <v>460</v>
+      </c>
+      <c r="O4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1970,16 +2051,25 @@
       <c r="L5" s="4" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>457</v>
+      </c>
+      <c r="N5" t="s">
+        <v>460</v>
+      </c>
+      <c r="O5" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
         <v>206</v>
       </c>
-      <c r="C6" t="s">
-        <v>455</v>
+      <c r="C6" s="3">
+        <v>37802</v>
       </c>
       <c r="D6">
         <v>22</v>
@@ -2005,8 +2095,17 @@
       <c r="L6" s="4" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>457</v>
+      </c>
+      <c r="N6" t="s">
+        <v>460</v>
+      </c>
+      <c r="O6" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2040,8 +2139,17 @@
       <c r="L7" s="4" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>457</v>
+      </c>
+      <c r="N7" t="s">
+        <v>460</v>
+      </c>
+      <c r="O7" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -2075,8 +2183,17 @@
       <c r="L8" s="4" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>457</v>
+      </c>
+      <c r="N8" t="s">
+        <v>460</v>
+      </c>
+      <c r="O8" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2089,7 +2206,7 @@
       <c r="D9">
         <v>32</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="7" t="s">
         <v>85</v>
       </c>
       <c r="F9" t="s">
@@ -2107,8 +2224,17 @@
       <c r="L9" s="4" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>457</v>
+      </c>
+      <c r="N9" t="s">
+        <v>460</v>
+      </c>
+      <c r="O9" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2137,8 +2263,17 @@
       <c r="L10" s="4" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>457</v>
+      </c>
+      <c r="N10" t="s">
+        <v>460</v>
+      </c>
+      <c r="O10" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>19</v>
       </c>
@@ -2172,8 +2307,17 @@
       <c r="L11" s="4" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="6" t="s">
+        <v>458</v>
+      </c>
+      <c r="N11" t="s">
+        <v>460</v>
+      </c>
+      <c r="O11" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -2210,8 +2354,17 @@
       <c r="L12" s="4" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>457</v>
+      </c>
+      <c r="N12" t="s">
+        <v>460</v>
+      </c>
+      <c r="O12" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -2245,8 +2398,17 @@
       <c r="L13" s="4" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>457</v>
+      </c>
+      <c r="N13" t="s">
+        <v>460</v>
+      </c>
+      <c r="O13" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -2283,8 +2445,17 @@
       <c r="L14" s="4" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>458</v>
+      </c>
+      <c r="N14" t="s">
+        <v>460</v>
+      </c>
+      <c r="O14" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>23</v>
       </c>
@@ -2318,8 +2489,17 @@
       <c r="L15" s="4" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>457</v>
+      </c>
+      <c r="N15" t="s">
+        <v>460</v>
+      </c>
+      <c r="O15" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -2350,9 +2530,17 @@
       <c r="J16" t="s">
         <v>249</v>
       </c>
-      <c r="L16" s="6"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>457</v>
+      </c>
+      <c r="N16" t="s">
+        <v>460</v>
+      </c>
+      <c r="O16" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -2380,9 +2568,17 @@
       <c r="I17" t="s">
         <v>252</v>
       </c>
-      <c r="L17" s="6"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>457</v>
+      </c>
+      <c r="N17" t="s">
+        <v>460</v>
+      </c>
+      <c r="O17" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -2410,9 +2606,17 @@
       <c r="I18" t="s">
         <v>260</v>
       </c>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>457</v>
+      </c>
+      <c r="N18" t="s">
+        <v>460</v>
+      </c>
+      <c r="O18" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -2446,8 +2650,17 @@
       <c r="L19" s="4" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>457</v>
+      </c>
+      <c r="N19" t="s">
+        <v>460</v>
+      </c>
+      <c r="O19" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -2475,8 +2688,17 @@
       <c r="I20" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>457</v>
+      </c>
+      <c r="N20" t="s">
+        <v>460</v>
+      </c>
+      <c r="O20" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -2513,8 +2735,17 @@
       <c r="L21" s="4" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>458</v>
+      </c>
+      <c r="N21" t="s">
+        <v>460</v>
+      </c>
+      <c r="O21" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -2545,8 +2776,17 @@
       <c r="L22" s="4" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>458</v>
+      </c>
+      <c r="N22" t="s">
+        <v>460</v>
+      </c>
+      <c r="O22" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -2580,8 +2820,17 @@
       <c r="L23" s="4" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>457</v>
+      </c>
+      <c r="N23" t="s">
+        <v>460</v>
+      </c>
+      <c r="O23" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -2609,8 +2858,17 @@
       <c r="I24" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>457</v>
+      </c>
+      <c r="N24" t="s">
+        <v>460</v>
+      </c>
+      <c r="O24" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -2644,8 +2902,17 @@
       <c r="K25" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>457</v>
+      </c>
+      <c r="N25" t="s">
+        <v>460</v>
+      </c>
+      <c r="O25" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -2679,8 +2946,17 @@
       <c r="L26" s="4" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>457</v>
+      </c>
+      <c r="N26" t="s">
+        <v>460</v>
+      </c>
+      <c r="O26" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2708,8 +2984,17 @@
       <c r="I27" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>457</v>
+      </c>
+      <c r="N27" t="s">
+        <v>460</v>
+      </c>
+      <c r="O27" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>36</v>
       </c>
@@ -2746,8 +3031,17 @@
       <c r="L28" s="4" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>457</v>
+      </c>
+      <c r="N28" t="s">
+        <v>460</v>
+      </c>
+      <c r="O28" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -2784,8 +3078,17 @@
       <c r="L29" s="4" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>457</v>
+      </c>
+      <c r="N29" t="s">
+        <v>460</v>
+      </c>
+      <c r="O29" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>38</v>
       </c>
@@ -2822,8 +3125,17 @@
       <c r="L30" s="4" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30" t="s">
+        <v>457</v>
+      </c>
+      <c r="N30" t="s">
+        <v>460</v>
+      </c>
+      <c r="O30" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -2851,8 +3163,17 @@
       <c r="L31" s="4" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>457</v>
+      </c>
+      <c r="N31" t="s">
+        <v>460</v>
+      </c>
+      <c r="O31" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>40</v>
       </c>
@@ -2889,8 +3210,17 @@
       <c r="L32" s="4" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>457</v>
+      </c>
+      <c r="N32" t="s">
+        <v>460</v>
+      </c>
+      <c r="O32" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>41</v>
       </c>
@@ -2927,8 +3257,17 @@
       <c r="L33" s="4" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>457</v>
+      </c>
+      <c r="N33" t="s">
+        <v>460</v>
+      </c>
+      <c r="O33" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>42</v>
       </c>
@@ -2965,8 +3304,17 @@
       <c r="L34" s="4" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>457</v>
+      </c>
+      <c r="N34" t="s">
+        <v>460</v>
+      </c>
+      <c r="O34" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>43</v>
       </c>
@@ -2994,8 +3342,17 @@
       <c r="L35" s="4" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M35" t="s">
+        <v>457</v>
+      </c>
+      <c r="N35" t="s">
+        <v>460</v>
+      </c>
+      <c r="O35" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>44</v>
       </c>
@@ -3032,8 +3389,17 @@
       <c r="L36" s="4" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>457</v>
+      </c>
+      <c r="N36" t="s">
+        <v>460</v>
+      </c>
+      <c r="O36" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>45</v>
       </c>
@@ -3062,8 +3428,17 @@
       <c r="L37" s="4" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>457</v>
+      </c>
+      <c r="N37" t="s">
+        <v>460</v>
+      </c>
+      <c r="O37" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>46</v>
       </c>
@@ -3100,8 +3475,17 @@
       <c r="L38" s="4" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38" t="s">
+        <v>457</v>
+      </c>
+      <c r="N38" t="s">
+        <v>460</v>
+      </c>
+      <c r="O38" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>47</v>
       </c>
@@ -3129,8 +3513,17 @@
       <c r="L39" s="4" t="s">
         <v>332</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M39" t="s">
+        <v>457</v>
+      </c>
+      <c r="N39" t="s">
+        <v>460</v>
+      </c>
+      <c r="O39" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -3167,8 +3560,17 @@
       <c r="L40" s="4" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>457</v>
+      </c>
+      <c r="N40" t="s">
+        <v>460</v>
+      </c>
+      <c r="O40" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>49</v>
       </c>
@@ -3205,8 +3607,17 @@
       <c r="L41" s="4" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
+        <v>457</v>
+      </c>
+      <c r="N41" t="s">
+        <v>460</v>
+      </c>
+      <c r="O41" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>50</v>
       </c>
@@ -3237,8 +3648,17 @@
       <c r="L42" s="4" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>457</v>
+      </c>
+      <c r="N42" t="s">
+        <v>460</v>
+      </c>
+      <c r="O42" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>51</v>
       </c>
@@ -3275,8 +3695,17 @@
       <c r="L43" s="4" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M43" t="s">
+        <v>457</v>
+      </c>
+      <c r="N43" t="s">
+        <v>460</v>
+      </c>
+      <c r="O43" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>52</v>
       </c>
@@ -3307,8 +3736,17 @@
       <c r="L44" s="4" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M44" t="s">
+        <v>457</v>
+      </c>
+      <c r="N44" t="s">
+        <v>460</v>
+      </c>
+      <c r="O44" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>53</v>
       </c>
@@ -3345,8 +3783,17 @@
       <c r="L45" s="4" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M45" t="s">
+        <v>457</v>
+      </c>
+      <c r="N45" t="s">
+        <v>460</v>
+      </c>
+      <c r="O45" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>54</v>
       </c>
@@ -3380,8 +3827,17 @@
       <c r="L46" s="4" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M46" t="s">
+        <v>457</v>
+      </c>
+      <c r="N46" t="s">
+        <v>460</v>
+      </c>
+      <c r="O46" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -3415,8 +3871,17 @@
       <c r="L47" s="4" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M47" t="s">
+        <v>457</v>
+      </c>
+      <c r="N47" t="s">
+        <v>460</v>
+      </c>
+      <c r="O47" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>56</v>
       </c>
@@ -3453,8 +3918,17 @@
       <c r="L48" s="4" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48" t="s">
+        <v>457</v>
+      </c>
+      <c r="N48" t="s">
+        <v>460</v>
+      </c>
+      <c r="O48" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>57</v>
       </c>
@@ -3491,8 +3965,17 @@
       <c r="L49" s="4" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M49" t="s">
+        <v>457</v>
+      </c>
+      <c r="N49" t="s">
+        <v>460</v>
+      </c>
+      <c r="O49" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>58</v>
       </c>
@@ -3526,8 +4009,17 @@
       <c r="L50" s="4" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50" t="s">
+        <v>457</v>
+      </c>
+      <c r="N50" t="s">
+        <v>460</v>
+      </c>
+      <c r="O50" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>59</v>
       </c>
@@ -3558,8 +4050,17 @@
       <c r="L51" s="4" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M51" t="s">
+        <v>457</v>
+      </c>
+      <c r="N51" t="s">
+        <v>460</v>
+      </c>
+      <c r="O51" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>60</v>
       </c>
@@ -3587,8 +4088,17 @@
       <c r="L52" s="4" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M52" t="s">
+        <v>457</v>
+      </c>
+      <c r="N52" t="s">
+        <v>460</v>
+      </c>
+      <c r="O52" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>61</v>
       </c>
@@ -3625,8 +4135,17 @@
       <c r="L53" s="4" t="s">
         <v>393</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M53" t="s">
+        <v>457</v>
+      </c>
+      <c r="N53" t="s">
+        <v>460</v>
+      </c>
+      <c r="O53" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>62</v>
       </c>
@@ -3657,8 +4176,17 @@
       <c r="L54" s="4" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54" t="s">
+        <v>457</v>
+      </c>
+      <c r="N54" t="s">
+        <v>460</v>
+      </c>
+      <c r="O54" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>63</v>
       </c>
@@ -3692,8 +4220,17 @@
       <c r="L55" s="4" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M55" t="s">
+        <v>457</v>
+      </c>
+      <c r="N55" t="s">
+        <v>460</v>
+      </c>
+      <c r="O55" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>64</v>
       </c>
@@ -3730,8 +4267,17 @@
       <c r="L56" s="4" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M56" t="s">
+        <v>457</v>
+      </c>
+      <c r="N56" t="s">
+        <v>460</v>
+      </c>
+      <c r="O56" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>65</v>
       </c>
@@ -3768,8 +4314,17 @@
       <c r="L57" s="4" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M57" t="s">
+        <v>457</v>
+      </c>
+      <c r="N57" t="s">
+        <v>460</v>
+      </c>
+      <c r="O57" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>66</v>
       </c>
@@ -3803,8 +4358,17 @@
       <c r="L58" s="4" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M58" t="s">
+        <v>457</v>
+      </c>
+      <c r="N58" t="s">
+        <v>460</v>
+      </c>
+      <c r="O58" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -3835,8 +4399,17 @@
       <c r="L59" s="4" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M59" t="s">
+        <v>457</v>
+      </c>
+      <c r="N59" t="s">
+        <v>460</v>
+      </c>
+      <c r="O59" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>68</v>
       </c>
@@ -3873,8 +4446,17 @@
       <c r="L60" s="4" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M60" t="s">
+        <v>457</v>
+      </c>
+      <c r="N60" t="s">
+        <v>460</v>
+      </c>
+      <c r="O60" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>69</v>
       </c>
@@ -3911,8 +4493,17 @@
       <c r="L61" s="4" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M61" t="s">
+        <v>457</v>
+      </c>
+      <c r="N61" t="s">
+        <v>460</v>
+      </c>
+      <c r="O61" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -3946,8 +4537,17 @@
       <c r="L62" s="4" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M62" t="s">
+        <v>457</v>
+      </c>
+      <c r="N62" t="s">
+        <v>460</v>
+      </c>
+      <c r="O62" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>71</v>
       </c>
@@ -3978,8 +4578,17 @@
       <c r="L63" s="4" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M63" t="s">
+        <v>457</v>
+      </c>
+      <c r="N63" t="s">
+        <v>460</v>
+      </c>
+      <c r="O63" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>72</v>
       </c>
@@ -4013,8 +4622,17 @@
       <c r="L64" s="4" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M64" t="s">
+        <v>457</v>
+      </c>
+      <c r="N64" t="s">
+        <v>460</v>
+      </c>
+      <c r="O64" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>73</v>
       </c>
@@ -4048,8 +4666,17 @@
       <c r="L65" s="4" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M65" t="s">
+        <v>457</v>
+      </c>
+      <c r="N65" t="s">
+        <v>460</v>
+      </c>
+      <c r="O65" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>74</v>
       </c>
@@ -4083,8 +4710,17 @@
       <c r="L66" s="4" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M66" t="s">
+        <v>457</v>
+      </c>
+      <c r="N66" t="s">
+        <v>460</v>
+      </c>
+      <c r="O66" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>75</v>
       </c>
@@ -4118,8 +4754,17 @@
       <c r="L67" s="4" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M67" t="s">
+        <v>457</v>
+      </c>
+      <c r="N67" t="s">
+        <v>460</v>
+      </c>
+      <c r="O67" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>76</v>
       </c>
@@ -4147,8 +4792,17 @@
       <c r="L68" s="4" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M68" t="s">
+        <v>457</v>
+      </c>
+      <c r="N68" t="s">
+        <v>460</v>
+      </c>
+      <c r="O68" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>77</v>
       </c>
@@ -4181,6 +4835,15 @@
       </c>
       <c r="L69" s="4" t="s">
         <v>454</v>
+      </c>
+      <c r="M69" t="s">
+        <v>457</v>
+      </c>
+      <c r="N69" t="s">
+        <v>460</v>
+      </c>
+      <c r="O69" t="s">
+        <v>461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>